<commit_message>
Succesful sms++-pypsa coupling with UCBlock only
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,7 +943,7 @@
         <v>50</v>
       </c>
       <c r="H3" s="1">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1004,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -1088,7 +1088,7 @@
         <v>50</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed inverse transformation for battery and hydro
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>solar</t>
   </si>
@@ -96,9 +96,6 @@
     <t>#210af5</t>
   </si>
   <si>
-    <t>air-sourced heat pump</t>
-  </si>
-  <si>
     <t>#0cdaf5</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>battery</t>
   </si>
   <si>
-    <t>onwind</t>
-  </si>
-  <si>
     <t>battery_link</t>
   </si>
   <si>
@@ -192,7 +186,22 @@
     <t>state_of_charge_initial</t>
   </si>
   <si>
-    <t>True</t>
+    <t>False</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>line 0-1</t>
+  </si>
+  <si>
+    <t>bus 1</t>
+  </si>
+  <si>
+    <t>demand 1</t>
   </si>
 </sst>
 </file>
@@ -516,7 +525,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +575,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -582,55 +591,55 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +682,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -685,6 +694,23 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
         <v>0.4</v>
       </c>
     </row>
@@ -695,10 +721,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +751,18 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -735,10 +772,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,22 +793,48 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -783,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -815,30 +878,28 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -847,7 +908,31 @@
         <v>1</v>
       </c>
       <c r="H2" s="1">
+        <v>100</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1">
         <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -882,10 +967,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -894,10 +979,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -912,7 +997,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,28 +1027,28 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
       <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
       <c r="L1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -996,13 +1081,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Succesfully implemented inverse transformation of lines
- Still to test for links
- Converted a completed network (not bad)
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>solar</t>
   </si>
@@ -156,9 +156,6 @@
     <t>e_init</t>
   </si>
   <si>
-    <t>p_nom_max</t>
-  </si>
-  <si>
     <t>battery</t>
   </si>
   <si>
@@ -193,6 +190,24 @@
   </si>
   <si>
     <t>hydro</t>
+  </si>
+  <si>
+    <t>bus 1</t>
+  </si>
+  <si>
+    <t>demand 1</t>
+  </si>
+  <si>
+    <t>line 0-1</t>
+  </si>
+  <si>
+    <t>bus 2</t>
+  </si>
+  <si>
+    <t>demand 2</t>
+  </si>
+  <si>
+    <t>line 1-2</t>
   </si>
 </sst>
 </file>
@@ -582,7 +597,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -590,7 +605,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -614,7 +629,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -622,7 +637,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -630,7 +645,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -643,10 +658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,6 +703,40 @@
         <v>0.4</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -695,10 +744,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,6 +777,28 @@
         <v>27</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -735,10 +806,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +842,59 @@
         <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +907,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,25 +941,25 @@
         <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -845,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -941,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
         <v>29</v>
@@ -956,13 +1079,13 @@
         <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1124,7 @@
         <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started reorder of the transfromation class
Added
- utils for common functions
- constants for constant attributes/dicts
- inverse for functions used in the inverse transformation
- io_parser for the solution file parsing
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -530,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +881,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,7 +985,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated up to iterate_blocks
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>solar</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>state_of_charge_initial</t>
-  </si>
-  <si>
-    <t>False</t>
   </si>
   <si>
     <t>wind</t>
@@ -565,7 +562,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -597,7 +594,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -629,7 +626,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -705,7 +702,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -722,7 +719,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -779,24 +776,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -847,7 +844,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -856,10 +853,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -880,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,10 +927,10 @@
         <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -948,16 +945,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -1034,13 +1031,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1">
         <v>-1</v>

</xml_diff>

<commit_message>
Updated to PyPSA package
Should work everything also from remote
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>solar</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>slack</t>
-  </si>
-  <si>
-    <t>False</t>
   </si>
 </sst>
 </file>
@@ -783,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,7 +833,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -848,7 +845,7 @@
         <v>20</v>
       </c>
       <c r="H2" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -863,7 +860,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -875,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -942,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,7 +1005,7 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
@@ -1026,7 +1023,7 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected thermalunit in inverse_transformation
Now statistics are correct for both investment and ucblock
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>solar</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>slack</t>
-  </si>
-  <si>
-    <t>False</t>
   </si>
   <si>
     <t>line 0-1</t>
@@ -654,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -699,7 +696,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -756,13 +753,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +772,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,7 +810,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -822,10 +819,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -834,7 +831,7 @@
         <v>0.1</v>
       </c>
       <c r="H2" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +896,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -911,7 +908,7 @@
         <v>20</v>
       </c>
       <c r="H2" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -923,10 +920,10 @@
         <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -938,7 +935,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1006,7 +1003,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1068,7 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
@@ -1089,7 +1086,7 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on investment errors and europe ucblock
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="115">
   <si>
     <t>solar</t>
   </si>
@@ -63,9 +63,6 @@
     <t>v_nom</t>
   </si>
   <si>
-    <t>demand 0</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>#66039c</t>
   </si>
   <si>
-    <t>bus 0</t>
-  </si>
-  <si>
     <t>p_max_pu</t>
   </si>
   <si>
@@ -192,25 +186,196 @@
     <t>slack</t>
   </si>
   <si>
-    <t>bus 1</t>
-  </si>
-  <si>
-    <t>demand 1</t>
-  </si>
-  <si>
-    <t>bus 2</t>
-  </si>
-  <si>
-    <t>battery_link 0-1</t>
-  </si>
-  <si>
-    <t>battery_link 1-2</t>
-  </si>
-  <si>
-    <t>demand 2</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>v_mag_pu_set</t>
+  </si>
+  <si>
+    <t>v_mag_pu_min</t>
+  </si>
+  <si>
+    <t>v_mag_pu_max</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>generator</t>
+  </si>
+  <si>
+    <t>sub_network</t>
+  </si>
+  <si>
+    <t>substation_off</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>substation_lv</t>
+  </si>
+  <si>
+    <t>IT0 0</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>IT1 0</t>
+  </si>
+  <si>
+    <t>relation/8185711-500-DC</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>relation/8185711</t>
+  </si>
+  <si>
+    <t>LINESTRING (8.306507186431089 40.84110865715793, 8.3065975 40.8410218, 8.3076221 40.8404009, 8.3106852 40.8424889, 8.3135283 40.8447798, 8.3138102 40.8452217, 8.3336448 40.8763037, 8.3547585 40.919545, 8.3629986 40.9246682, 8.438959 40.9365347, 8.4637641 40.9377018, 8.4968945 40.9423702, 8.578777 40.9519001, 8.6672684 40.9695948, 8.7741276 41.0055206, 8.7916373 41.0131954, 8.8120433 41.0387725, 8.8171498 41.1805441, 8.9698212 41.2809838, 10.4425021 41.516806, 12.771601 41.3438287, 12.8105575 41.4138493, 12.8113675 41.429471, 12.8075105 41.4306293, 12.806985991114674 41.42980383291617)</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>build_year</t>
+  </si>
+  <si>
+    <t>lifetime</t>
+  </si>
+  <si>
+    <t>p_nom_mod</t>
+  </si>
+  <si>
+    <t>p_nom_max</t>
+  </si>
+  <si>
+    <t>p_set</t>
+  </si>
+  <si>
+    <t>capital_cost</t>
+  </si>
+  <si>
+    <t>marginal_cost</t>
+  </si>
+  <si>
+    <t>marginal_cost_quadratic</t>
+  </si>
+  <si>
+    <t>stand_by_cost</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>terrain_factor</t>
+  </si>
+  <si>
+    <t>committable</t>
+  </si>
+  <si>
+    <t>start_up_cost</t>
+  </si>
+  <si>
+    <t>shut_down_cost</t>
+  </si>
+  <si>
+    <t>min_up_time</t>
+  </si>
+  <si>
+    <t>min_down_time</t>
+  </si>
+  <si>
+    <t>up_time_before</t>
+  </si>
+  <si>
+    <t>down_time_before</t>
+  </si>
+  <si>
+    <t>ramp_limit_up</t>
+  </si>
+  <si>
+    <t>ramp_limit_down</t>
+  </si>
+  <si>
+    <t>ramp_limit_start_up</t>
+  </si>
+  <si>
+    <t>ramp_limit_shut_down</t>
+  </si>
+  <si>
+    <t>p_nom_opt</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>geometry</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>project_status</t>
+  </si>
+  <si>
+    <t>under_construction</t>
+  </si>
+  <si>
+    <t>underground</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>underwater_fraction</t>
+  </si>
+  <si>
+    <t>start_line_idx</t>
+  </si>
+  <si>
+    <t>end_line_idx</t>
+  </si>
+  <si>
+    <t>e_sum_max</t>
+  </si>
+  <si>
+    <t>q_set</t>
+  </si>
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>bus_idx</t>
+  </si>
+  <si>
+    <t>IT0 0 CCGT</t>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>IT1 0 0 solar</t>
   </si>
 </sst>
 </file>
@@ -547,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -555,7 +720,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -563,95 +728,95 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -661,10 +826,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G1" sqref="G1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,72 +837,139 @@
     <col min="1" max="7" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="1">
+        <v>380</v>
+      </c>
+      <c r="D2" s="1">
+        <v>11.861807419676801</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43.502700216278299</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1">
+        <v>380</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.7398246778425897</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40.032889929774797</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.4</v>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -747,10 +979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,35 +1003,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -830,22 +1051,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -855,105 +1076,326 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="N1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <v>39535.519999999997</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2">
+        <v>39535.519999999997</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N2">
+        <v>54.725344874286201</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
-        <v>200</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I4" s="1"/>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2">
+        <v>110915.226328986</v>
+      </c>
+      <c r="T2">
+        <v>0.52684054680077297</v>
+      </c>
+      <c r="U2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <v>1153.4058162686799</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3">
+        <v>1153.4058162686799</v>
+      </c>
+      <c r="F3">
+        <v>38969.282766677301</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0.01</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>35</v>
+      </c>
+      <c r="S3">
+        <v>54744.164802564301</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -962,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:AS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,93 +1418,278 @@
     <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="H2" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="I2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="I3" s="1">
-        <v>100</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="1">
+        <v>31000</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>51869.6104378526</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>464.56899717447197</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>500</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>0.96184305038492401</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1071,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,60 +1731,28 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
       <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
-        <v>45</v>
-      </c>
       <c r="L1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2">
-        <v>0.95</v>
-      </c>
-      <c r="G2">
-        <v>0.95</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>100</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1170,7 +1765,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,13 +1785,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added merged_links in direct transformation
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="135">
   <si>
     <t>solar</t>
   </si>
@@ -144,9 +144,6 @@
     <t>efficiency</t>
   </si>
   <si>
-    <t>e_init</t>
-  </si>
-  <si>
     <t>battery</t>
   </si>
   <si>
@@ -375,7 +372,70 @@
     <t>CCGT</t>
   </si>
   <si>
-    <t>IT1 0 0 solar</t>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>e_sum_min</t>
+  </si>
+  <si>
+    <t>PQ</t>
+  </si>
+  <si>
+    <t>IT0 0 biomass</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>e_nom_mod</t>
+  </si>
+  <si>
+    <t>e_nom_min</t>
+  </si>
+  <si>
+    <t>e_nom_max</t>
+  </si>
+  <si>
+    <t>e_min_pu</t>
+  </si>
+  <si>
+    <t>e_max_pu</t>
+  </si>
+  <si>
+    <t>e_initial</t>
+  </si>
+  <si>
+    <t>e_initial_per_period</t>
+  </si>
+  <si>
+    <t>e_cyclic</t>
+  </si>
+  <si>
+    <t>e_cyclic_per_period</t>
+  </si>
+  <si>
+    <t>marginal_cost_storage</t>
+  </si>
+  <si>
+    <t>e_nom_opt</t>
+  </si>
+  <si>
+    <t>IT0 0 H2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>IT0 0 H2 Electrolysis</t>
+  </si>
+  <si>
+    <t>H2 electrolysis</t>
+  </si>
+  <si>
+    <t>IT0 0 H2 Fuel Cell</t>
+  </si>
+  <si>
+    <t>H2 fuel cell</t>
   </si>
 </sst>
 </file>
@@ -733,7 +793,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -765,7 +825,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -773,7 +833,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -797,7 +857,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -805,7 +865,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -813,7 +873,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -826,10 +886,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:Q1048576"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -857,42 +917,42 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1">
         <v>380</v>
@@ -914,10 +974,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -925,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -933,7 +993,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1">
         <v>380</v>
@@ -955,10 +1015,10 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -966,10 +1026,45 @@
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>11.861807419676801</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43.502700216278299</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1003,24 +1098,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1161,7 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1076,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,312 +1185,348 @@
     <col min="4" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK1" t="s">
         <v>109</v>
       </c>
-      <c r="M1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" t="s">
-        <v>85</v>
-      </c>
-      <c r="V1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W1" t="s">
-        <v>87</v>
-      </c>
-      <c r="X1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AL1" t="s">
         <v>95</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AM1" t="s">
         <v>110</v>
       </c>
-      <c r="AH1" t="s">
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2">
+        <v>395</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2">
+        <v>39535.519999999997</v>
+      </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="e">
+        <f t="shared" ref="M2:M3" si="0">-inf</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>112</v>
       </c>
-      <c r="B2" t="s">
+      <c r="R2">
+        <v>54.725344874286201</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
         <v>63</v>
       </c>
-      <c r="C2">
+      <c r="W2">
+        <v>110915.226328986</v>
+      </c>
+      <c r="X2">
+        <v>0.52684054680077297</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
         <v>39535.519999999997</v>
       </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2">
-        <v>39535.519999999997</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2">
-        <v>54.725344874286201</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>64</v>
-      </c>
-      <c r="S2">
-        <v>110915.226328986</v>
-      </c>
-      <c r="T2">
-        <v>0.52684054680077297</v>
-      </c>
-      <c r="U2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
-        <v>1</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="AM2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3">
-        <v>1153.4058162686799</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3"/>
       <c r="E3">
-        <v>1153.4058162686799</v>
+        <v>384</v>
       </c>
       <c r="F3">
-        <v>38969.282766677301</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
+        <v>384</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0.01</v>
+        <v>0</v>
+      </c>
+      <c r="M3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>117</v>
       </c>
       <c r="R3">
-        <v>35</v>
+        <v>15.8282051282051</v>
       </c>
       <c r="S3">
-        <v>54744.164802564301</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>63</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>294201.05117025401</v>
       </c>
       <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>69</v>
       </c>
       <c r="Z3">
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3">
         <v>0</v>
       </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
       <c r="AE3">
         <v>1</v>
       </c>
       <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
-        <v>1</v>
-      </c>
-      <c r="AH3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>384</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1404,18 +1535,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS3"/>
+  <dimension ref="A1:AS4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="31" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1429,7 +1562,7 @@
         <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1438,31 +1571,31 @@
         <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>5</v>
@@ -1471,114 +1604,114 @@
         <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="J2" s="1">
         <v>1000</v>
@@ -1587,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M2" s="1">
         <v>1000</v>
@@ -1623,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y2" s="1">
         <v>0</v>
@@ -1653,10 +1786,10 @@
         <v>1000</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="AL2" s="1">
         <v>1</v>
@@ -1681,15 +1814,212 @@
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.57730000000000004</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>251621.03444133099</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>132325.720604876</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>2</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1731,7 +2061,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
@@ -1746,13 +2076,13 @@
         <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1762,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1774,24 +2104,180 @@
     <col min="4" max="4" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
+      <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>222.485403385334</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Treat generators as intermittentblocks
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -1156,7 +1156,7 @@
   <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="e">
-        <f t="shared" ref="M2:M3" si="0">-inf</f>
+        <f t="shared" ref="M2" si="0">-inf</f>
         <v>#NAME?</v>
       </c>
       <c r="N2" t="s">
@@ -1415,7 +1415,7 @@
   <dimension ref="A1:AS2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,7 +1764,7 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Modified conversion to account batteries properly
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Carrier"/>
@@ -116,13 +116,13 @@
     <t>H2</t>
   </si>
   <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
     <t>True</t>
-  </si>
-  <si>
-    <t>inf</t>
-  </si>
-  <si>
-    <t>False</t>
   </si>
   <si>
     <t>p_nom_extendable</t>
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3">
         <v>19711.8691837313</v>
@@ -1431,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U2" s="2">
         <v>0</v>
@@ -1440,13 +1440,13 @@
         <v>35</v>
       </c>
       <c r="W2" s="3">
-        <v>54744.1648025643</v>
+        <v>55</v>
       </c>
       <c r="X2" s="2">
         <v>1</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Z2" s="2">
         <v>0</v>
@@ -1499,7 +1499,7 @@
   </sheetPr>
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1705,7 +1705,7 @@
         <v>0.5773</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M2" s="2">
         <v>100</v>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Y2" s="2">
         <v>0</v>
@@ -1820,7 +1820,7 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M3" s="2">
         <v>100</v>
@@ -1871,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Y3" s="2">
         <v>0</v>
@@ -1997,7 +1997,7 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2133,7 +2133,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -2157,13 +2157,13 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P2" s="2">
         <v>0</v>
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Y2" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Reduced snapshots for Antonio
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\sms\transformation_pypsa_smspp\test\configs\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Carrier" sheetId="1" r:id="rId1"/>
-    <sheet name="Bus" sheetId="2" r:id="rId2"/>
-    <sheet name="Load" sheetId="3" r:id="rId3"/>
-    <sheet name="Line" sheetId="4" r:id="rId4"/>
-    <sheet name="Generator" sheetId="5" r:id="rId5"/>
-    <sheet name="Link" sheetId="6" r:id="rId6"/>
-    <sheet name="StorageUnit" sheetId="7" r:id="rId7"/>
-    <sheet name="Store" sheetId="8" r:id="rId8"/>
+    <sheet r:id="rId1" sheetId="1" name="Carrier"/>
+    <sheet r:id="rId2" sheetId="2" name="Bus"/>
+    <sheet r:id="rId3" sheetId="3" name="Load"/>
+    <sheet r:id="rId4" sheetId="4" name="Line"/>
+    <sheet r:id="rId5" sheetId="5" name="Generator"/>
+    <sheet r:id="rId6" sheetId="6" name="Link"/>
+    <sheet r:id="rId7" sheetId="7" name="StorageUnit"/>
+    <sheet r:id="rId8" sheetId="8" name="Store"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -121,13 +116,13 @@
     <t>H2</t>
   </si>
   <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
     <t>False</t>
-  </si>
-  <si>
-    <t>inf</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
   <si>
     <t>p_nom_extendable</t>
@@ -412,7 +407,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,67 +452,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -527,10 +526,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -568,71 +567,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -660,7 +659,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -683,11 +682,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -696,13 +695,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -712,7 +711,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -721,7 +720,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -730,7 +729,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -738,10 +737,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -814,13 +813,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,7 +827,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -836,7 +835,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -844,7 +843,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
@@ -852,7 +851,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -860,7 +859,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>112</v>
       </c>
@@ -868,7 +867,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>114</v>
       </c>
@@ -876,7 +875,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>116</v>
       </c>
@@ -884,7 +883,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>118</v>
       </c>
@@ -892,7 +891,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>120</v>
       </c>
@@ -900,7 +899,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -908,7 +907,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>124</v>
       </c>
@@ -916,7 +915,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
@@ -924,7 +923,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>126</v>
       </c>
@@ -946,24 +945,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="18" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="7" t="s">
         <v>74</v>
       </c>
@@ -1025,10 +1028,10 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="8">
-        <v>11.861807419676801</v>
+        <v>11.8618074196768</v>
       </c>
       <c r="E2" s="8">
-        <v>43.502700216278299</v>
+        <v>43.5027002162783</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>90</v>
@@ -1059,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
@@ -1068,10 +1071,10 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8">
-        <v>11.861807419676801</v>
+        <v>11.8618074196768</v>
       </c>
       <c r="E3" s="8">
-        <v>43.502700216278299</v>
+        <v>43.5027002162783</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>30</v>
@@ -1114,12 +1117,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="7" t="s">
         <v>74</v>
       </c>
@@ -1155,14 +1160,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1200,37 +1210,52 @@
   </sheetPr>
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="32" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="8.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -1349,7 +1374,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -1361,16 +1386,16 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3">
-        <v>19711.869183731302</v>
+        <v>19711.8691837313</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3">
-        <v>19711.869183731302</v>
+        <v>19711.8691837313</v>
       </c>
       <c r="I2" s="3">
         <v>725545.55299179</v>
@@ -1384,9 +1409,8 @@
       <c r="L2" s="2">
         <v>0</v>
       </c>
-      <c r="M2" s="15" t="e">
+      <c r="M2" s="15">
         <f>-inf</f>
-        <v>#NAME?</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>32</v>
@@ -1407,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U2" s="2">
         <v>0</v>
@@ -1422,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Z2" s="2">
         <v>0</v>
@@ -1457,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="AL2" s="3">
-        <v>62875.819329802704</v>
+        <v>62875.8193298027</v>
       </c>
       <c r="AM2" s="2">
         <v>0</v>
@@ -1477,35 +1501,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="23" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1687,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -1657,10 +1702,10 @@
         <v>75</v>
       </c>
       <c r="F2" s="3">
-        <v>0.57730000000000004</v>
+        <v>0.5773</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -1675,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M2" s="2">
         <v>100</v>
@@ -1693,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="3">
-        <v>251621.03444133099</v>
+        <v>251621.034441331</v>
       </c>
       <c r="S2" s="2">
         <v>0</v>
@@ -1711,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Y2" s="2">
         <v>0</v>
@@ -1757,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -1775,7 +1820,7 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
@@ -1790,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M3" s="2">
         <v>100</v>
@@ -1826,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Y3" s="2">
         <v>0</v>
@@ -1886,21 +1931,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="30.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1950,30 +1997,42 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2062,7 +2121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -2080,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -2098,13 +2157,13 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P2" s="2">
         <v>0</v>
@@ -2131,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Y2" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Fallback for inverse transformation
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="121">
   <si>
     <t>name</t>
   </si>
@@ -115,12 +115,6 @@
     <t>bus_idx</t>
   </si>
   <si>
-    <t>IT0 0 H2</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
     <t>False</t>
   </si>
   <si>
@@ -247,19 +241,7 @@
     <t>end_line_idx</t>
   </si>
   <si>
-    <t>IT0 0 H2 Electrolysis</t>
-  </si>
-  <si>
     <t>IT0 0</t>
-  </si>
-  <si>
-    <t>H2 electrolysis</t>
-  </si>
-  <si>
-    <t>IT0 0 H2 Fuel Cell</t>
-  </si>
-  <si>
-    <t>H2 fuel cell</t>
   </si>
   <si>
     <t>Generator</t>
@@ -825,111 +807,111 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -944,7 +926,9 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -968,57 +952,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="O1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="P1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9">
         <v>380</v>
@@ -1031,7 +1015,7 @@
         <v>43.502700216278299</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -1042,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -1053,51 +1037,29 @@
         <v>1</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="Q2" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
+      <c r="A3" s="7"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="8">
-        <v>11.861807419676801</v>
-      </c>
-      <c r="E3" s="8">
-        <v>43.502700216278299</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="9">
-        <v>1</v>
-      </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="7" t="s">
-        <v>104</v>
-      </c>
+      <c r="P3" s="7"/>
       <c r="Q3" s="2"/>
     </row>
   </sheetData>
@@ -1132,13 +1094,13 @@
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1170,22 +1132,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1232,46 +1194,46 @@
   <sheetData>
     <row r="1" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O1" s="14" t="s">
         <v>16</v>
@@ -1301,49 +1263,49 @@
         <v>21</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AD1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AE1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AF1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AG1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AH1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AK1" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL1" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="AJ1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="AM1" s="14" t="s">
         <v>28</v>
@@ -1351,13 +1313,13 @@
     </row>
     <row r="2" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3">
@@ -1367,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3">
         <v>19711.869183731302</v>
@@ -1389,7 +1351,7 @@
         <v>#NAME?</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -1398,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="R2" s="3">
         <v>0.01</v>
@@ -1407,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U2" s="2">
         <v>0</v>
@@ -1422,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z2" s="2">
         <v>0</v>
@@ -1475,7 +1437,9 @@
   </sheetPr>
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1510,10 +1474,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
@@ -1522,7 +1486,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>23</v>
@@ -1534,28 +1498,28 @@
         <v>25</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R1" s="8" t="s">
         <v>21</v>
@@ -1567,181 +1531,117 @@
         <v>19</v>
       </c>
       <c r="U1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="X1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Z1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AB1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AD1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AE1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AF1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AG1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AH1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AK1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AL1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AM1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AN1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AO1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AP1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AR1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AS1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AR1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS1" s="9" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="2" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.57730000000000004</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="2">
-        <v>100</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="2">
-        <v>100</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="3">
-        <v>251621.03444133099</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>0</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-      <c r="AG2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>0</v>
-      </c>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="2"/>
@@ -1750,113 +1650,45 @@
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
       <c r="AQ2" s="3"/>
-      <c r="AR2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="2">
-        <v>2</v>
-      </c>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
     </row>
     <row r="3" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="2">
-        <v>100</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="2">
-        <v>100</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>1</v>
-      </c>
-      <c r="R3" s="3">
-        <v>132325.720604876</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2">
-        <v>0</v>
-      </c>
-      <c r="W3" s="2">
-        <v>1</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>0</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>0</v>
-      </c>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="2"/>
@@ -1865,12 +1697,8 @@
       <c r="AO3" s="2"/>
       <c r="AP3" s="2"/>
       <c r="AQ3" s="3"/>
-      <c r="AR3" s="2">
-        <v>2</v>
-      </c>
-      <c r="AS3" s="2">
-        <v>0</v>
-      </c>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1911,16 +1739,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
@@ -1929,13 +1757,13 @@
         <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1950,8 +1778,8 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,91 +1891,35 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3">
-        <v>222.485403385334</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>10</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>2</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated to PyPSA 1.0 (no retrofit)
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -1,32 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\sms\transformation_pypsa_smspp\test\configs\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Carrier" sheetId="1" r:id="rId1"/>
-    <sheet name="Bus" sheetId="2" r:id="rId2"/>
-    <sheet name="Load" sheetId="3" r:id="rId3"/>
-    <sheet name="Line" sheetId="4" r:id="rId4"/>
-    <sheet name="Generator" sheetId="5" r:id="rId5"/>
-    <sheet name="Link" sheetId="6" r:id="rId6"/>
-    <sheet name="StorageUnit" sheetId="7" r:id="rId7"/>
-    <sheet name="Store" sheetId="8" r:id="rId8"/>
+    <sheet r:id="rId1" sheetId="1" name="Carrier"/>
+    <sheet r:id="rId2" sheetId="2" name="Bus"/>
+    <sheet r:id="rId3" sheetId="3" name="Load"/>
+    <sheet r:id="rId4" sheetId="4" name="Line"/>
+    <sheet r:id="rId5" sheetId="5" name="Generator"/>
+    <sheet r:id="rId6" sheetId="6" name="Link"/>
+    <sheet r:id="rId7" sheetId="7" name="StorageUnit"/>
+    <sheet r:id="rId8" sheetId="8" name="Store"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -115,6 +110,12 @@
     <t>bus_idx</t>
   </si>
   <si>
+    <t>IT0 0 H2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
     <t>False</t>
   </si>
   <si>
@@ -241,7 +242,19 @@
     <t>end_line_idx</t>
   </si>
   <si>
+    <t>IT0 0 H2 Electrolysis</t>
+  </si>
+  <si>
     <t>IT0 0</t>
+  </si>
+  <si>
+    <t>H2 electrolysis</t>
+  </si>
+  <si>
+    <t>IT0 0 H2 Fuel Cell</t>
+  </si>
+  <si>
+    <t>H2 fuel cell</t>
   </si>
   <si>
     <t>Generator</t>
@@ -394,7 +407,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,67 +452,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -509,10 +526,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -550,71 +567,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -642,7 +659,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -665,11 +682,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -678,13 +695,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -694,7 +711,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -703,7 +720,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -712,7 +729,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -720,10 +737,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -796,122 +813,122 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -926,96 +943,98 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="18" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B2" s="9">
         <v>380</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="8">
-        <v>11.861807419676801</v>
+        <v>11.8618074196768</v>
       </c>
       <c r="E2" s="8">
-        <v>43.502700216278299</v>
+        <v>43.5027002162783</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -1026,10 +1045,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -1037,29 +1056,51 @@
         <v>1</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q2" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="9"/>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="8">
+        <v>11.86</v>
+      </c>
+      <c r="E3" s="8">
+        <v>43.5</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="7"/>
+      <c r="P3" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="Q3" s="2"/>
     </row>
   </sheetData>
@@ -1076,12 +1117,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1092,15 +1135,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1117,14 +1160,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1132,22 +1180,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1164,76 +1212,91 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="32" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="8.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="O1" s="14" t="s">
         <v>16</v>
@@ -1263,76 +1326,76 @@
         <v>21</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Z1" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AB1" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AC1" s="14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AD1" s="14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AE1" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AF1" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AI1" s="14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AJ1" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AK1" s="14" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AL1" s="13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AM1" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="3">
-        <v>19711.869183731302</v>
+        <v>19711.8691837313</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3">
-        <v>19711.869183731302</v>
+        <v>19711.8691837313</v>
       </c>
       <c r="I2" s="3">
         <v>725545.55299179</v>
@@ -1346,12 +1409,11 @@
       <c r="L2" s="2">
         <v>0</v>
       </c>
-      <c r="M2" s="15" t="e">
+      <c r="M2" s="15">
         <f>-inf</f>
-        <v>#NAME?</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -1360,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="R2" s="3">
         <v>0.01</v>
@@ -1369,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U2" s="2">
         <v>0</v>
@@ -1384,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Z2" s="2">
         <v>0</v>
@@ -1419,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="AL2" s="3">
-        <v>62875.819329802704</v>
+        <v>62875.8193298027</v>
       </c>
       <c r="AM2" s="2">
         <v>0</v>
@@ -1437,47 +1499,66 @@
   </sheetPr>
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="23" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
@@ -1486,7 +1567,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>23</v>
@@ -1498,28 +1579,28 @@
         <v>25</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R1" s="8" t="s">
         <v>21</v>
@@ -1531,117 +1612,181 @@
         <v>19</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AA1" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AC1" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AF1" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AK1" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AL1" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AM1" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AN1" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AO1" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AP1" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AQ1" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AR1" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AS1" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
+      <c r="E2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.58</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2">
+        <v>100</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>251621.03</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0</v>
+      </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
+      <c r="AG2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>0</v>
+      </c>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="2"/>
@@ -1650,45 +1795,113 @@
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
       <c r="AQ2" s="3"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
-    </row>
-    <row r="3" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="AR2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
+      <c r="E3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2">
+        <v>100</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3">
+        <v>132325.72</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>0</v>
+      </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
+      <c r="AG3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>0</v>
+      </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="2"/>
@@ -1697,8 +1910,12 @@
       <c r="AO3" s="2"/>
       <c r="AP3" s="2"/>
       <c r="AQ3" s="3"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
+      <c r="AR3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1714,21 +1931,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="30.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1739,16 +1958,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
@@ -1757,13 +1976,13 @@
         <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1778,30 +1997,42 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1890,36 +2121,92 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2">
+        <v>100</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>222.49</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small analysis tools - sector coupled network
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Carrier"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -809,9 +809,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -925,9 +925,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1997,7 +2021,7 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Added DesignNetworkBlock - direct transformation
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:AS3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1719,7 +1719,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="3">
-        <v>251621.03</v>
+        <v>250</v>
       </c>
       <c r="S2" s="2">
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="R3" s="3">
-        <v>132325.72</v>
+        <v>250</v>
       </c>
       <c r="S3" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Updated tests/corrected multi-links dimensions
</commit_message>
<xml_diff>
--- a/test/configs/data/components.xlsx
+++ b/test/configs/data/components.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\sms\transformation_pypsa_smspp\test\configs\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Carrier"/>
-    <sheet r:id="rId2" sheetId="2" name="Bus"/>
-    <sheet r:id="rId3" sheetId="3" name="Load"/>
-    <sheet r:id="rId4" sheetId="4" name="Line"/>
-    <sheet r:id="rId5" sheetId="5" name="Generator"/>
-    <sheet r:id="rId6" sheetId="6" name="Link"/>
-    <sheet r:id="rId7" sheetId="7" name="StorageUnit"/>
-    <sheet r:id="rId8" sheetId="8" name="Store"/>
+    <sheet name="Carrier" sheetId="1" r:id="rId1"/>
+    <sheet name="Bus" sheetId="2" r:id="rId2"/>
+    <sheet name="Load" sheetId="3" r:id="rId3"/>
+    <sheet name="Line" sheetId="4" r:id="rId4"/>
+    <sheet name="Generator" sheetId="5" r:id="rId5"/>
+    <sheet name="Link" sheetId="6" r:id="rId6"/>
+    <sheet name="StorageUnit" sheetId="7" r:id="rId7"/>
+    <sheet name="Store" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -407,8 +412,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,73 +456,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -529,10 +530,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -570,71 +571,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -662,7 +663,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -685,11 +686,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -698,13 +699,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -714,7 +715,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -723,7 +724,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -732,7 +733,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -740,10 +741,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -816,13 +817,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="21.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,7 +831,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -838,7 +839,7 @@
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -846,7 +847,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
@@ -854,7 +855,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
@@ -862,7 +863,7 @@
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>112</v>
       </c>
@@ -870,7 +871,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>114</v>
       </c>
@@ -878,7 +879,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>116</v>
       </c>
@@ -886,7 +887,7 @@
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>118</v>
       </c>
@@ -894,7 +895,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>120</v>
       </c>
@@ -902,7 +903,7 @@
         <v>121</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -910,7 +911,7 @@
         <v>123</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>124</v>
       </c>
@@ -918,7 +919,7 @@
         <v>123</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
@@ -926,7 +927,7 @@
         <v>123</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -934,7 +935,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -942,7 +943,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -950,7 +951,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
@@ -972,28 +973,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="17" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="17" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="8.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1043,7 @@
         <v>102</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>74</v>
       </c>
@@ -1055,10 +1052,10 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="10">
-        <v>11.8618074196768</v>
+        <v>11.861807419676801</v>
       </c>
       <c r="E2" s="10">
-        <v>43.5027002162783</v>
+        <v>43.502700216278299</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>90</v>
@@ -1089,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
@@ -1144,14 +1141,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="17" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="17" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="8.88671875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>74</v>
       </c>
@@ -1187,19 +1182,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="4" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1239,50 +1229,35 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="8.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="32" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -1401,7 +1376,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -1413,7 +1388,7 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="4">
-        <v>19711.8691837313</v>
+        <v>19711.869183731302</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1422,7 +1397,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="4">
-        <v>19711.8691837313</v>
+        <v>19711.869183731302</v>
       </c>
       <c r="I2" s="4">
         <v>725545.55299179</v>
@@ -1436,8 +1411,9 @@
       <c r="L2" s="2">
         <v>0</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="16" t="e">
         <f>-inf</f>
+        <v>#NAME?</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>32</v>
@@ -1508,7 +1484,7 @@
         <v>1</v>
       </c>
       <c r="AL2" s="4">
-        <v>62875.8193298027</v>
+        <v>62875.819329802704</v>
       </c>
       <c r="AM2" s="2">
         <v>0</v>
@@ -1526,58 +1502,37 @@
   </sheetPr>
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="13" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="8" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="43" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1669,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -1729,7 +1684,7 @@
         <v>75</v>
       </c>
       <c r="F2" s="4">
-        <v>0.58</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -1829,7 +1784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -1958,23 +1913,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="30.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2024,42 +1977,29 @@
   </sheetPr>
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2148,7 +2088,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>